<commit_message>
Atualizar mês de Maio
</commit_message>
<xml_diff>
--- a/preco_investido.xlsx
+++ b/preco_investido.xlsx
@@ -94,25 +94,25 @@
     <t>TSLA34</t>
   </si>
   <si>
+    <t>AAPL34</t>
+  </si>
+  <si>
+    <t>C1BS34</t>
+  </si>
+  <si>
+    <t>MGLU3</t>
+  </si>
+  <si>
+    <t>CPFF11</t>
+  </si>
+  <si>
+    <t>ITSA2F</t>
+  </si>
+  <si>
+    <t>VALE3F</t>
+  </si>
+  <si>
     <t>COCA34</t>
-  </si>
-  <si>
-    <t>AAPL34</t>
-  </si>
-  <si>
-    <t>C1BS34</t>
-  </si>
-  <si>
-    <t>MGLU3</t>
-  </si>
-  <si>
-    <t>CPFF11</t>
-  </si>
-  <si>
-    <t>ITSA2F</t>
-  </si>
-  <si>
-    <t>VALE3F</t>
   </si>
 </sst>
 </file>
@@ -503,7 +503,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>25.89815789473684</v>
+        <v>73.66131578947369</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -525,7 +525,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>11.42179577464789</v>
+        <v>12.88067375886525</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -547,7 +547,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>48.14358974358975</v>
+        <v>47.89415584415585</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -558,7 +558,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>40.96424242424242</v>
+        <v>74.83722222222222</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -569,7 +569,7 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>60.46777777777778</v>
+        <v>110.8544444444444</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -580,7 +580,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>9.220490797546013</v>
+        <v>9.422576687116566</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -591,7 +591,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>12.81181818181818</v>
+        <v>19.29623376623377</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -613,7 +613,7 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>22.51629032258064</v>
+        <v>24.54693548387097</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -624,7 +624,7 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>7.337178423236516</v>
+        <v>7.709543568464731</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -635,7 +635,7 @@
         <v>15</v>
       </c>
       <c r="C15">
-        <v>196.541</v>
+        <v>217.563</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -646,7 +646,7 @@
         <v>16</v>
       </c>
       <c r="C16">
-        <v>71.86871794871796</v>
+        <v>150.7195555555556</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -657,7 +657,7 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>132.8005555555555</v>
+        <v>160.1547619047619</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -668,7 +668,7 @@
         <v>18</v>
       </c>
       <c r="C18">
-        <v>62.544</v>
+        <v>103.6566129032258</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -679,7 +679,7 @@
         <v>19</v>
       </c>
       <c r="C19">
-        <v>15.44117647058824</v>
+        <v>38.10470588235294</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -690,7 +690,7 @@
         <v>20</v>
       </c>
       <c r="C20">
-        <v>19.94833333333333</v>
+        <v>22.19833333333333</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -745,7 +745,7 @@
         <v>25</v>
       </c>
       <c r="C25">
-        <v>28.6746511627907</v>
+        <v>32.17232558139535</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -756,7 +756,7 @@
         <v>26</v>
       </c>
       <c r="C26">
-        <v>53.74763636363637</v>
+        <v>51.18026315789474</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -767,7 +767,7 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>46.07455882352942</v>
+        <v>68.45352941176471</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -778,7 +778,7 @@
         <v>28</v>
       </c>
       <c r="C28">
-        <v>61.64529411764706</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -789,7 +789,7 @@
         <v>29</v>
       </c>
       <c r="C29">
-        <v>2.14</v>
+        <v>72.45333333333333</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -800,7 +800,7 @@
         <v>30</v>
       </c>
       <c r="C30">
-        <v>41.43047619047619</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -811,7 +811,7 @@
         <v>31</v>
       </c>
       <c r="C31">
-        <v>2.98</v>
+        <v>54.62790697674419</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -822,7 +822,7 @@
         <v>32</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>65.58620689655173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>